<commit_message>
Update Team Meetings - Updated.xlsx
updated attendance
</commit_message>
<xml_diff>
--- a/Team Meetings - Updated.xlsx
+++ b/Team Meetings - Updated.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cnkeng/Desktop/fall 2020 classes/Software Design/Excel Sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cnkeng/Desktop/fall 2020 classes/Software Design/Software-Design-Artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9620C5B-3008-FE48-9881-3078FE8EBB24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95DDCCB-F85A-CB49-8E11-EBD98F20CF59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20660" xr2:uid="{B69BAA51-2B07-4930-841B-9107909D754E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25040" windowHeight="20660" xr2:uid="{B69BAA51-2B07-4930-841B-9107909D754E}"/>
   </bookViews>
   <sheets>
     <sheet name="TeamF" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
   <si>
     <t>Contact Info</t>
   </si>
@@ -192,13 +192,19 @@
   </si>
   <si>
     <t>Everyone agreed to learn Git and also make some edits/comments/issues in the Jira project to show that they have access to it</t>
+  </si>
+  <si>
+    <t>Everyone is going to make a comment or create an issue to show that they have access to the Jira project, if they haven't done so already</t>
+  </si>
+  <si>
+    <t>Repeat of yesterday's meeting for those who couldn't attend</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -266,6 +272,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -321,7 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -372,6 +384,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -382,6 +397,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -705,7 +721,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I13" sqref="I13"/>
+      <selection pane="topRight" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -717,69 +733,70 @@
     <col min="5" max="5" width="17.5" customWidth="1"/>
     <col min="6" max="6" width="16.5" customWidth="1"/>
     <col min="7" max="7" width="18.1640625" customWidth="1"/>
-    <col min="8" max="18" width="11" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="9" max="18" width="11" customWidth="1"/>
     <col min="19" max="29" width="12.6640625" customWidth="1"/>
     <col min="30" max="34" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:48" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="32" t="s">
+      <c r="C2" s="34"/>
+      <c r="D2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
       <c r="H2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="32" t="s">
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="32" t="s">
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="33"/>
-      <c r="AA2" s="32" t="s">
+      <c r="V2" s="34"/>
+      <c r="W2" s="34"/>
+      <c r="X2" s="34"/>
+      <c r="Y2" s="34"/>
+      <c r="Z2" s="34"/>
+      <c r="AA2" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
-      <c r="AF2" s="33"/>
-      <c r="AG2" s="33"/>
-      <c r="AH2" s="33"/>
-      <c r="AI2" s="33"/>
+      <c r="AB2" s="34"/>
+      <c r="AC2" s="34"/>
+      <c r="AD2" s="34"/>
+      <c r="AE2" s="34"/>
+      <c r="AF2" s="34"/>
+      <c r="AG2" s="34"/>
+      <c r="AH2" s="34"/>
+      <c r="AI2" s="34"/>
       <c r="AJ2" s="3"/>
       <c r="AK2" s="3"/>
       <c r="AL2" s="3"/>
@@ -936,7 +953,9 @@
       <c r="G4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="23"/>
+      <c r="H4" s="23" t="s">
+        <v>10</v>
+      </c>
       <c r="I4" s="23"/>
       <c r="J4" s="23"/>
       <c r="K4" s="23"/>
@@ -985,7 +1004,9 @@
         <v>10</v>
       </c>
       <c r="G5" s="22"/>
-      <c r="H5" s="23"/>
+      <c r="H5" s="23" t="s">
+        <v>10</v>
+      </c>
       <c r="I5" s="23"/>
       <c r="J5" s="23"/>
       <c r="K5" s="23"/>
@@ -1034,7 +1055,9 @@
       <c r="G6" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="23"/>
+      <c r="H6" s="23" t="s">
+        <v>10</v>
+      </c>
       <c r="I6" s="23"/>
       <c r="J6" s="23"/>
       <c r="K6" s="23"/>
@@ -1076,14 +1099,16 @@
       <c r="D7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="35" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="22"/>
-      <c r="H7" s="23"/>
+      <c r="H7" s="23" t="s">
+        <v>10</v>
+      </c>
       <c r="I7" s="23"/>
       <c r="J7" s="23"/>
       <c r="K7" s="23"/>
@@ -1134,7 +1159,7 @@
       <c r="G8" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="23"/>
+      <c r="H8" s="22"/>
       <c r="I8" s="23"/>
       <c r="J8" s="23"/>
       <c r="K8" s="23"/>
@@ -1185,7 +1210,9 @@
       <c r="G9" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="23"/>
+      <c r="H9" s="23" t="s">
+        <v>10</v>
+      </c>
       <c r="I9" s="23"/>
       <c r="J9" s="23"/>
       <c r="K9" s="23"/>
@@ -1227,7 +1254,7 @@
       <c r="D10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="35" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="23" t="s">
@@ -1236,7 +1263,9 @@
       <c r="G10" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="23"/>
+      <c r="H10" s="35" t="s">
+        <v>11</v>
+      </c>
       <c r="I10" s="23"/>
       <c r="J10" s="23"/>
       <c r="K10" s="23"/>
@@ -1282,9 +1311,10 @@
       <c r="G13" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="H13" s="26"/>
+      <c r="H13" s="29" t="s">
+        <v>53</v>
+      </c>
       <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
       <c r="K13" s="26"/>
       <c r="L13" s="26"/>
       <c r="M13" s="26"/>
@@ -1328,9 +1358,11 @@
       <c r="G14" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="H14" s="27"/>
+      <c r="H14" s="29" t="s">
+        <v>51</v>
+      </c>
       <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
+      <c r="J14"/>
       <c r="K14" s="27"/>
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
@@ -1352,8 +1384,8 @@
       <c r="AC14" s="27"/>
       <c r="AD14" s="27"/>
       <c r="AE14" s="27"/>
-      <c r="AF14" s="29"/>
-      <c r="AG14" s="30"/>
+      <c r="AF14" s="30"/>
+      <c r="AG14" s="31"/>
       <c r="AH14" s="27"/>
       <c r="AI14" s="27"/>
       <c r="AJ14" s="7"/>
@@ -1370,7 +1402,7 @@
       <c r="AU14" s="7"/>
       <c r="AV14" s="7"/>
     </row>
-    <row r="15" spans="1:48" s="9" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:48" s="9" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A15" s="17" t="s">
         <v>41</v>
       </c>
@@ -1385,9 +1417,11 @@
         <v>45</v>
       </c>
       <c r="G15" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="H15" s="27"/>
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
       <c r="K15" s="27"/>
@@ -1445,7 +1479,9 @@
       <c r="G16" s="26">
         <v>5</v>
       </c>
-      <c r="H16" s="26"/>
+      <c r="H16" s="26">
+        <v>5</v>
+      </c>
       <c r="I16" s="26"/>
       <c r="J16" s="26"/>
       <c r="K16" s="26"/>

</xml_diff>

<commit_message>
don't need the extra Mac file
</commit_message>
<xml_diff>
--- a/Team Meetings - Updated.xlsx
+++ b/Team Meetings - Updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cnkeng/Desktop/fall 2020 classes/Software Design/Software-Design-Artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1332CD9-7254-B24F-B264-77F36EE80A44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA17B058-2709-244C-855B-F7D67176870D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20660" xr2:uid="{B69BAA51-2B07-4930-841B-9107909D754E}"/>
   </bookViews>
@@ -755,7 +755,7 @@
   </sheetPr>
   <dimension ref="A1:AV23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="J15" sqref="J15"/>
     </sheetView>

</xml_diff>